<commit_message>
analysis dps3xx fixed point solution
</commit_message>
<xml_diff>
--- a/documents/analysis/dps3xx compensating calculation.xlsx
+++ b/documents/analysis/dps3xx compensating calculation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Oversampling Rate</t>
   </si>
@@ -141,6 +141,9 @@
     <t>Dec Value</t>
   </si>
   <si>
+    <t>Reg. Bitwidth</t>
+  </si>
+  <si>
     <t>Temperature Polynomial</t>
   </si>
   <si>
@@ -199,6 +202,45 @@
   </si>
   <si>
     <t>FFFFF924</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>device-&gt;coes.c00</t>
+  </si>
+  <si>
+    <t>scaled_pressure * (device-&gt;coes.c10 + scaled_pressure *(device-&gt;coes.c20 + scaled_pressure * device-&gt;coes.c30))</t>
+  </si>
+  <si>
+    <t>scaled_pressure * device-&gt;coes.c30</t>
+  </si>
+  <si>
+    <t>+ device-&gt;coes.c20</t>
+  </si>
+  <si>
+    <t>* scaled_pressure</t>
+  </si>
+  <si>
+    <t>+ device-&gt;coes.c10</t>
+  </si>
+  <si>
+    <t>scaled_temperature * device-&gt;coes.c01</t>
+  </si>
+  <si>
+    <t>scaled_temperature * scaled_pressure * (device-&gt;coes.c11 + scaled_pressure * device-&gt;coes.c21)</t>
+  </si>
+  <si>
+    <t>scaled_pressure * device-&gt;coes.c21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ device-&gt;coes.c11 </t>
+  </si>
+  <si>
+    <t>* scaled_temperature * scaled_pressure</t>
+  </si>
+  <si>
+    <t>final value:</t>
   </si>
 </sst>
 </file>
@@ -206,10 +248,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -242,6 +284,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -263,6 +312,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -275,6 +332,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -302,29 +367,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -334,6 +376,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,30 +412,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,25 +440,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,7 +584,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,155 +602,155 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="22">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -640,21 +802,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -666,11 +813,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,17 +843,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,142 +871,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -854,69 +1016,114 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1240,213 +1447,213 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="24.7777777777778" style="14" customWidth="1"/>
-    <col min="2" max="2" width="22.8888888888889" style="14" customWidth="1"/>
-    <col min="3" max="3" width="17" style="14" customWidth="1"/>
-    <col min="4" max="4" width="23.8888888888889" style="14" customWidth="1"/>
-    <col min="5" max="5" width="19" style="14" customWidth="1"/>
-    <col min="6" max="6" width="38.5555555555556" style="14" customWidth="1"/>
-    <col min="7" max="16384" width="8.88888888888889" style="14"/>
+    <col min="1" max="1" width="24.7777777777778" style="28" customWidth="1"/>
+    <col min="2" max="2" width="22.8888888888889" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17" style="28" customWidth="1"/>
+    <col min="4" max="4" width="23.8888888888889" style="28" customWidth="1"/>
+    <col min="5" max="5" width="19" style="28" customWidth="1"/>
+    <col min="6" max="6" width="38.5555555555556" style="28" customWidth="1"/>
+    <col min="7" max="16384" width="8.88888888888889" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="1" spans="1:6">
-      <c r="A1" s="15" t="s">
+    <row r="1" s="28" customFormat="1" spans="1:6">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="31">
         <v>524288</v>
       </c>
-      <c r="C2" s="18" t="str">
+      <c r="C2" s="31" t="str">
         <f>DEC2HEX(B2)</f>
         <v>80000</v>
       </c>
-      <c r="D2" s="18" t="str">
+      <c r="D2" s="31" t="str">
         <f>DEC2BIN(B2/65536,8)&amp;DEC2BIN(MOD(B2,65536)/256,8)&amp;DEC2BIN(MOD(B2,256),8)</f>
         <v>000010000000000000000000</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="31">
         <v>1572864</v>
       </c>
-      <c r="C3" s="18" t="str">
+      <c r="C3" s="31" t="str">
         <f t="shared" ref="C3:C9" si="0">DEC2HEX(B3)</f>
         <v>180000</v>
       </c>
-      <c r="D3" s="18" t="str">
+      <c r="D3" s="31" t="str">
         <f t="shared" ref="D3:D9" si="1">DEC2BIN(B3/65536,8)&amp;DEC2BIN(MOD(B3,65536)/256,8)&amp;DEC2BIN(MOD(B3,256),8)</f>
         <v>000110000000000000000000</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="31">
         <v>3670016</v>
       </c>
-      <c r="C4" s="18" t="str">
+      <c r="C4" s="31" t="str">
         <f t="shared" si="0"/>
         <v>380000</v>
       </c>
-      <c r="D4" s="18" t="str">
+      <c r="D4" s="31" t="str">
         <f t="shared" si="1"/>
         <v>001110000000000000000000</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="31">
         <v>7864320</v>
       </c>
-      <c r="C5" s="18" t="str">
+      <c r="C5" s="31" t="str">
         <f t="shared" si="0"/>
         <v>780000</v>
       </c>
-      <c r="D5" s="18" t="str">
+      <c r="D5" s="31" t="str">
         <f t="shared" si="1"/>
         <v>011110000000000000000000</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="31">
         <v>253952</v>
       </c>
-      <c r="C6" s="18" t="str">
+      <c r="C6" s="31" t="str">
         <f t="shared" si="0"/>
         <v>3E000</v>
       </c>
-      <c r="D6" s="18" t="str">
+      <c r="D6" s="31" t="str">
         <f t="shared" si="1"/>
         <v>000000111110000000000000</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="31">
         <v>516096</v>
       </c>
-      <c r="C7" s="18" t="str">
+      <c r="C7" s="31" t="str">
         <f t="shared" si="0"/>
         <v>7E000</v>
       </c>
-      <c r="D7" s="18" t="str">
+      <c r="D7" s="31" t="str">
         <f t="shared" si="1"/>
         <v>000001111110000000000000</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="31">
         <v>1040384</v>
       </c>
-      <c r="C8" s="18" t="str">
+      <c r="C8" s="31" t="str">
         <f t="shared" si="0"/>
         <v>FE000</v>
       </c>
-      <c r="D8" s="18" t="str">
+      <c r="D8" s="31" t="str">
         <f t="shared" si="1"/>
         <v>000011111110000000000000</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="31">
         <v>2088960</v>
       </c>
-      <c r="C9" s="18" t="str">
+      <c r="C9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>1FE000</v>
       </c>
-      <c r="D9" s="18" t="str">
-        <f>DEC2BIN(B9/65536,8)&amp;DEC2BIN(MOD(B9,65536)/256,8)&amp;DEC2BIN(MOD(B9,256),8)</f>
+      <c r="D9" s="31" t="str">
+        <f t="shared" si="1"/>
         <v>000111111110000000000000</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="30" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1459,348 +1666,635 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="26.562962962963" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.1111111111111" style="1" customWidth="1"/>
-    <col min="4" max="5" width="21.8888888888889" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="1" width="33.6666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1111111111111" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1111111111111" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.8888888888889" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1111111111111" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.1111111111111" style="1"/>
+    <col min="10" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="6" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="9"/>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="7" t="s">
+      <c r="C6" s="9"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="9">
         <v>152376</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9">
-        <f>HEX2DEC(25338)</f>
-        <v>152376</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="9">
         <f>B7/B6</f>
         <v>0.295247395833333</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="10">
-        <f>D7/B6</f>
-        <v>0.295247395833333</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="7" t="s">
+      <c r="C10" s="9"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="9">
         <v>-409061</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="7" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="9">
         <f>B11/B10</f>
         <v>-0.393182709461122</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="6" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E14" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="6" t="s">
+      <c r="F14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="11" t="s">
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="9">
-        <f>IF(HEX2DEC(B17)&gt;2147483647,HEX2DEC(B17)-4294967296,HEX2DEC(B17))</f>
+      <c r="B15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="11">
+        <f>IF(HEX2DEC(B15)&gt;2147483647,HEX2DEC(B15)-4294967296,HEX2DEC(B15))</f>
         <v>222</v>
       </c>
-      <c r="D17" s="9">
-        <f>C17*0.5</f>
+      <c r="D15" s="13">
+        <v>12</v>
+      </c>
+      <c r="E15" s="11">
+        <f>C15*0.5</f>
         <v>111</v>
       </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="11" t="s">
+      <c r="F15" s="12"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="9">
-        <f t="shared" ref="C18:C25" si="0">IF(HEX2DEC(B18)&gt;2147483647,HEX2DEC(B18)-4294967296,HEX2DEC(B18))</f>
+      <c r="B16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" ref="C16:C23" si="0">IF(HEX2DEC(B16)&gt;2147483647,HEX2DEC(B16)-4294967296,HEX2DEC(B16))</f>
         <v>-295</v>
       </c>
-      <c r="D18" s="9">
-        <f>B8*C18</f>
-        <v>-87.0979817708333</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="11" t="s">
+      <c r="D16" s="13">
+        <v>12</v>
+      </c>
+      <c r="E16" s="11">
+        <f>B8*C16</f>
+        <v>-87.0979817708332</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="9">
+      <c r="B17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="11">
         <f t="shared" si="0"/>
         <v>82580</v>
       </c>
-      <c r="E19" s="12">
+      <c r="D17" s="13">
+        <v>20</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12">
         <v>82580</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="11" t="s">
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="9">
+      <c r="B18" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="11">
         <f t="shared" si="0"/>
         <v>-55343</v>
       </c>
-      <c r="E20" s="12">
-        <f>C20*B12</f>
+      <c r="D18" s="13">
+        <v>20</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12">
+        <f>C18*B12</f>
         <v>21759.9106897069</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="11" t="s">
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="9">
+      <c r="B19" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="11">
         <f t="shared" si="0"/>
         <v>-3496</v>
       </c>
-      <c r="E21" s="12">
-        <f>C21*B8</f>
+      <c r="D19" s="13">
+        <v>16</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12">
+        <f>C19*B8</f>
         <v>-1032.18489583333</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="20" t="s">
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="9">
+      <c r="B20" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="11">
         <f t="shared" si="0"/>
         <v>1545</v>
       </c>
-      <c r="E22" s="12">
-        <f>C22*B8*B12</f>
-        <v>-179.353134280115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="D20" s="13">
+        <v>16</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12">
+        <f>C20*B8*B12</f>
+        <v>-179.353134280114</v>
+      </c>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="9">
+      <c r="B21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="11">
         <f t="shared" si="0"/>
         <v>-11412</v>
       </c>
-      <c r="E23" s="12">
-        <f>-C23*B12*B12</f>
-        <v>1764.21124213499</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="D21" s="13">
+        <v>16</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12">
+        <f>C21*B12*B12</f>
+        <v>-1764.21124213499</v>
+      </c>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="9">
+      <c r="B22" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="11">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="E24" s="12">
-        <f>C24*B12*B12*B8</f>
-        <v>9.85890425754407</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="11" t="s">
+      <c r="D22" s="13">
+        <v>16</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12">
+        <f>C22*B12*B12*B8</f>
+        <v>9.85890425754406</v>
+      </c>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="9">
+      <c r="B23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="11">
         <f t="shared" si="0"/>
         <v>-1756</v>
       </c>
-      <c r="E25" s="12">
-        <f>C25*B12*B12*B12</f>
+      <c r="D23" s="13">
+        <v>16</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12">
+        <f>C23*B12*B12*B12</f>
         <v>106.735218854292</v>
       </c>
-    </row>
-    <row r="26" spans="4:5">
-      <c r="D26" s="9">
-        <f>SUM(D17:D25)</f>
-        <v>23.9020182291667</v>
-      </c>
-      <c r="E26" s="9">
-        <f>SUM(E17:E25)</f>
-        <v>105009.17802484</v>
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11">
+        <f>SUM(E15:E23)</f>
+        <v>23.9020182291668</v>
+      </c>
+      <c r="F24" s="11">
+        <f>SUM(F15:F23)</f>
+        <v>101480.75554057</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="21">
+        <f>C17</f>
+        <v>82580</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="11">
+        <f>B12*C23</f>
+        <v>690.42883781373</v>
+      </c>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="22">
+        <f>C21</f>
+        <v>-11412</v>
+      </c>
+      <c r="F30" s="11">
+        <f>F29+C21</f>
+        <v>-10721.5711621863</v>
+      </c>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="22">
+        <f>B12</f>
+        <v>-0.393182709461122</v>
+      </c>
+      <c r="F31" s="11">
+        <f>F30*B12</f>
+        <v>4215.53639922863</v>
+      </c>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="22">
+        <f>C18</f>
+        <v>-55343</v>
+      </c>
+      <c r="F32" s="11">
+        <f>F31+C18</f>
+        <v>-51127.4636007714</v>
+      </c>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="22">
+        <f>B12</f>
+        <v>-0.393182709461122</v>
+      </c>
+      <c r="F33" s="11">
+        <f>F32*B12</f>
+        <v>20102.4346664262</v>
+      </c>
+      <c r="G33" s="11">
+        <f>F33</f>
+        <v>20102.4346664262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="11">
+        <f>B8*C19</f>
+        <v>-1032.18489583333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="11">
+        <f>B12*C22</f>
+        <v>-84.9274652436024</v>
+      </c>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="11">
+        <f>F36+C20</f>
+        <v>1460.0725347564</v>
+      </c>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="11">
+        <f>F37*B12*B8</f>
+        <v>-169.49423002257</v>
+      </c>
+      <c r="G38" s="11">
+        <f>F38</f>
+        <v>-169.49423002257</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="11">
+        <f>SUM(G27:G38)</f>
+        <v>101480.75554057</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A39:F39"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
create a new folder: utilities
</commit_message>
<xml_diff>
--- a/documents/analysis/dps3xx compensating calculation.xlsx
+++ b/documents/analysis/dps3xx compensating calculation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Oversampling Rate</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>Scale Factor(Hex)</t>
+  </si>
+  <si>
+    <t>BitWidth(Singned)</t>
   </si>
   <si>
     <t>Scale Factor(Power)</t>
@@ -247,12 +250,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.000000000_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -275,21 +279,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -300,13 +289,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,17 +309,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,16 +340,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -375,7 +365,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,9 +401,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,20 +422,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -440,19 +444,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,151 +606,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,7 +777,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -782,48 +786,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,9 +808,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -866,157 +846,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1057,13 +1061,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1077,13 +1075,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1098,9 +1090,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1110,14 +1099,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1444,217 +1433,245 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="24.7777777777778" style="28" customWidth="1"/>
-    <col min="2" max="2" width="22.8888888888889" style="28" customWidth="1"/>
-    <col min="3" max="3" width="17" style="28" customWidth="1"/>
-    <col min="4" max="4" width="23.8888888888889" style="28" customWidth="1"/>
-    <col min="5" max="5" width="19" style="28" customWidth="1"/>
-    <col min="6" max="6" width="38.5555555555556" style="28" customWidth="1"/>
-    <col min="7" max="16384" width="8.88888888888889" style="28"/>
+    <col min="1" max="1" width="24.7777777777778" style="23" customWidth="1"/>
+    <col min="2" max="2" width="22.8888888888889" style="23" customWidth="1"/>
+    <col min="3" max="3" width="17" style="23" customWidth="1"/>
+    <col min="4" max="4" width="23.8888888888889" style="23" customWidth="1"/>
+    <col min="5" max="5" width="17" style="23" customWidth="1"/>
+    <col min="6" max="6" width="19" style="23" customWidth="1"/>
+    <col min="7" max="7" width="38.5555555555556" style="23" customWidth="1"/>
+    <col min="8" max="16384" width="8.88888888888889" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" s="28" customFormat="1" spans="1:6">
-      <c r="A1" s="29" t="s">
+    <row r="1" s="23" customFormat="1" spans="1:7">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="30" t="s">
+      <c r="G1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="31">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="26">
         <v>524288</v>
       </c>
-      <c r="C2" s="31" t="str">
+      <c r="C2" s="26" t="str">
         <f>DEC2HEX(B2)</f>
         <v>80000</v>
       </c>
-      <c r="D2" s="31" t="str">
+      <c r="D2" s="26" t="str">
         <f>DEC2BIN(B2/65536,8)&amp;DEC2BIN(MOD(B2,65536)/256,8)&amp;DEC2BIN(MOD(B2,256),8)</f>
         <v>000010000000000000000000</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="32">
+      <c r="E2" s="27">
+        <v>21</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="31">
+    <row r="3" spans="1:7">
+      <c r="A3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="26">
         <v>1572864</v>
       </c>
-      <c r="C3" s="31" t="str">
+      <c r="C3" s="26" t="str">
         <f t="shared" ref="C3:C9" si="0">DEC2HEX(B3)</f>
         <v>180000</v>
       </c>
-      <c r="D3" s="31" t="str">
+      <c r="D3" s="26" t="str">
         <f t="shared" ref="D3:D9" si="1">DEC2BIN(B3/65536,8)&amp;DEC2BIN(MOD(B3,65536)/256,8)&amp;DEC2BIN(MOD(B3,256),8)</f>
         <v>000110000000000000000000</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="32">
+      <c r="E3" s="27">
+        <v>22</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="31">
+    <row r="4" spans="1:7">
+      <c r="A4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="26">
         <v>3670016</v>
       </c>
-      <c r="C4" s="31" t="str">
+      <c r="C4" s="26" t="str">
         <f t="shared" si="0"/>
         <v>380000</v>
       </c>
-      <c r="D4" s="31" t="str">
+      <c r="D4" s="26" t="str">
         <f t="shared" si="1"/>
         <v>001110000000000000000000</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="32">
+      <c r="E4" s="27">
+        <v>23</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="31">
+    <row r="5" spans="1:7">
+      <c r="A5" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="26">
         <v>7864320</v>
       </c>
-      <c r="C5" s="31" t="str">
+      <c r="C5" s="26" t="str">
         <f t="shared" si="0"/>
         <v>780000</v>
       </c>
-      <c r="D5" s="31" t="str">
+      <c r="D5" s="26" t="str">
         <f t="shared" si="1"/>
         <v>011110000000000000000000</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="32">
+      <c r="E5" s="27">
+        <v>24</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="31">
+    <row r="6" spans="1:7">
+      <c r="A6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="26">
         <v>253952</v>
       </c>
-      <c r="C6" s="31" t="str">
+      <c r="C6" s="26" t="str">
         <f t="shared" si="0"/>
         <v>3E000</v>
       </c>
-      <c r="D6" s="31" t="str">
-        <f t="shared" si="1"/>
+      <c r="D6" s="26" t="str">
+        <f>DEC2BIN(B6/65536,8)&amp;DEC2BIN(MOD(B6,65536)/256,8)&amp;DEC2BIN(MOD(B6,256),8)</f>
         <v>000000111110000000000000</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="27">
+        <v>19</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="30" t="s">
+      <c r="G6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="31">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="26">
         <v>516096</v>
       </c>
-      <c r="C7" s="31" t="str">
+      <c r="C7" s="26" t="str">
         <f t="shared" si="0"/>
         <v>7E000</v>
       </c>
-      <c r="D7" s="31" t="str">
+      <c r="D7" s="26" t="str">
         <f t="shared" si="1"/>
         <v>000001111110000000000000</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="30" t="s">
+      <c r="E7" s="27">
+        <v>20</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="31">
+      <c r="G7" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="26">
         <v>1040384</v>
       </c>
-      <c r="C8" s="31" t="str">
+      <c r="C8" s="26" t="str">
         <f t="shared" si="0"/>
         <v>FE000</v>
       </c>
-      <c r="D8" s="31" t="str">
+      <c r="D8" s="26" t="str">
         <f t="shared" si="1"/>
         <v>000011111110000000000000</v>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="30" t="s">
+      <c r="E8" s="27">
+        <v>21</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="31">
+      <c r="G8" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="26">
         <v>2088960</v>
       </c>
-      <c r="C9" s="31" t="str">
+      <c r="C9" s="26" t="str">
         <f t="shared" si="0"/>
         <v>1FE000</v>
       </c>
-      <c r="D9" s="31" t="str">
+      <c r="D9" s="26" t="str">
         <f t="shared" si="1"/>
         <v>000111111110000000000000</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>15</v>
+      <c r="E9" s="27">
+        <v>22</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1668,8 +1685,8 @@
   <sheetPr/>
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18"/>
@@ -1680,14 +1697,14 @@
     <col min="4" max="4" width="13.1111111111111" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.8888888888889" style="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1111111111111" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1111111111111" style="1" customWidth="1"/>
     <col min="8" max="9" width="12.1111111111111" style="1"/>
     <col min="10" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1696,11 +1713,11 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="24"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1709,11 +1726,11 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="25"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1722,7 +1739,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="26"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="8"/>
@@ -1733,44 +1750,41 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="E5" s="19"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="17"/>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="9">
         <v>152376</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E7" s="17"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="9">
         <f>B7/B6</f>
@@ -1778,53 +1792,52 @@
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="17"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="17"/>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="C10" s="9" t="str">
+        <f>"0x"&amp;DEC2HEX(B10,8)</f>
+        <v>0x000FE000</v>
+      </c>
+      <c r="E10" s="17"/>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="9">
         <v>-409061</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="9">
         <f>B11/B10</f>
@@ -1832,8 +1845,7 @@
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="17"/>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7">
@@ -1841,42 +1853,41 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="17"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="11">
         <f>IF(HEX2DEC(B15)&gt;2147483647,HEX2DEC(B15)-4294967296,HEX2DEC(B15))</f>
         <v>222</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="9">
         <v>12</v>
       </c>
       <c r="E15" s="11">
@@ -1884,20 +1895,20 @@
         <v>111</v>
       </c>
       <c r="F15" s="12"/>
-      <c r="J15" s="27"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="11">
         <f t="shared" ref="C16:C23" si="0">IF(HEX2DEC(B16)&gt;2147483647,HEX2DEC(B16)-4294967296,HEX2DEC(B16))</f>
         <v>-295</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="9">
         <v>12</v>
       </c>
       <c r="E16" s="11">
@@ -1905,40 +1916,40 @@
         <v>-87.0979817708332</v>
       </c>
       <c r="F16" s="12"/>
-      <c r="J16" s="27"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="11">
         <f t="shared" si="0"/>
         <v>82580</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="9">
         <v>20</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="12">
         <v>82580</v>
       </c>
-      <c r="J17" s="27"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" s="11">
         <f t="shared" si="0"/>
         <v>-55343</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="9">
         <v>20</v>
       </c>
       <c r="E18" s="11"/>
@@ -1946,20 +1957,20 @@
         <f>C18*B12</f>
         <v>21759.9106897069</v>
       </c>
-      <c r="J18" s="27"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="11">
         <f t="shared" si="0"/>
         <v>-3496</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="9">
         <v>16</v>
       </c>
       <c r="E19" s="11"/>
@@ -1967,20 +1978,20 @@
         <f>C19*B8</f>
         <v>-1032.18489583333</v>
       </c>
-      <c r="J19" s="27"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="33" t="s">
         <v>55</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>56</v>
       </c>
       <c r="C20" s="11">
         <f t="shared" si="0"/>
         <v>1545</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="9">
         <v>16</v>
       </c>
       <c r="E20" s="11"/>
@@ -1988,20 +1999,20 @@
         <f>C20*B8*B12</f>
         <v>-179.353134280114</v>
       </c>
-      <c r="J20" s="27"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="11">
         <f t="shared" si="0"/>
         <v>-11412</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="9">
         <v>16</v>
       </c>
       <c r="E21" s="11"/>
@@ -2009,20 +2020,20 @@
         <f>C21*B12*B12</f>
         <v>-1764.21124213499</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22" s="11">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="9">
         <v>16</v>
       </c>
       <c r="E22" s="11"/>
@@ -2030,20 +2041,20 @@
         <f>C22*B12*B12*B8</f>
         <v>9.85890425754406</v>
       </c>
-      <c r="J22" s="27"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="11">
         <f t="shared" si="0"/>
         <v>-1756</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="9">
         <v>16</v>
       </c>
       <c r="E23" s="11"/>
@@ -2051,12 +2062,12 @@
         <f>C23*B12*B12*B12</f>
         <v>106.735218854292</v>
       </c>
-      <c r="J23" s="27"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11">
         <f>SUM(E15:E23)</f>
@@ -2068,46 +2079,46 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13" t="s">
-        <v>62</v>
+      <c r="A26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="21">
+      <c r="A27" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13">
         <f>C17</f>
         <v>82580</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
+      <c r="A28" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2120,13 +2131,13 @@
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="22">
+      <c r="A30" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13">
         <f>C21</f>
         <v>-11412</v>
       </c>
@@ -2137,13 +2148,13 @@
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="22">
+      <c r="A31" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13">
         <f>B12</f>
         <v>-0.393182709461122</v>
       </c>
@@ -2154,13 +2165,13 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="22">
+      <c r="A32" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13">
         <f>C18</f>
         <v>-55343</v>
       </c>
@@ -2171,13 +2182,13 @@
       <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="22">
+      <c r="A33" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13">
         <f>B12</f>
         <v>-0.393182709461122</v>
       </c>
@@ -2191,38 +2202,38 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="A34" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="11">
         <f>B8*C19</f>
         <v>-1032.18489583333</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
+      <c r="A35" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
+      <c r="A36" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
       <c r="F36" s="11">
         <f>B12*C22</f>
         <v>-84.9274652436024</v>
@@ -2230,13 +2241,13 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
+      <c r="A37" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
       <c r="F37" s="11">
         <f>F36+C20</f>
         <v>1460.0725347564</v>
@@ -2244,13 +2255,13 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
+      <c r="A38" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
       <c r="F38" s="11">
         <f>F37*B12*B8</f>
         <v>-169.49423002257</v>
@@ -2261,14 +2272,14 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="23"/>
+      <c r="A39" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="11">
         <f>SUM(G27:G38)</f>
         <v>101480.75554057</v>

</xml_diff>